<commit_message>
Bauluz updates and others
</commit_message>
<xml_diff>
--- a/data-input/data-quality/data-quality.xlsx
+++ b/data-input/data-quality/data-quality.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t>iso</t>
   </si>
@@ -639,6 +639,24 @@
   </si>
   <si>
     <t>ZW</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>GQ</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>ZZ</t>
+  </si>
+  <si>
+    <t>QF</t>
   </si>
 </sst>
 </file>
@@ -704,8 +722,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:B204" totalsRowShown="0">
-  <autoFilter ref="A1:B204"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:B210" totalsRowShown="0">
+  <autoFilter ref="A1:B210"/>
   <sortState ref="A2:B84">
     <sortCondition ref="A1:A84"/>
   </sortState>
@@ -980,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B204"/>
+  <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1453,7 +1471,7 @@
         <v>98</v>
       </c>
       <c r="B58" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -2622,6 +2640,54 @@
       </c>
       <c r="B204" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B205" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B206" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B207" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B208" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B209" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B210" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020 update - part 1
I am importing new data sent by ccordinator; this requires removing old ones and insuring that there are no duplicates
</commit_message>
<xml_diff>
--- a/data-input/data-quality/data-quality.xlsx
+++ b/data-input/data-quality/data-quality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasblanchet/GitHub/wid-world/data-input/data-quality/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowaidakhaled/Documents/GitHub/wid-world/data-input/data-quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DFCEE6-0C8B-C344-B11F-CBA4D41002D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D3B7A8-1E21-6949-8930-F7B237769093}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25300" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9120" yWindow="-21880" windowWidth="25300" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
   <si>
     <t>iso</t>
   </si>
@@ -661,6 +661,60 @@
   </si>
   <si>
     <t>XM-MER</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>KZ</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>UZ</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>JP</t>
   </si>
 </sst>
 </file>
@@ -726,8 +780,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:B211" totalsRowShown="0">
-  <autoFilter ref="A1:B211" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:B229" totalsRowShown="0">
+  <autoFilter ref="A1:B229" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:B84">
     <sortCondition ref="A1:A84"/>
   </sortState>
@@ -1002,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2702,6 +2756,150 @@
         <v>3</v>
       </c>
     </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B212" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B213" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B214" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B215" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B216" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B217" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B218" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B219" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B220" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B221" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B222" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B223" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B224" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B225" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B226" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B227" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B228" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B229" s="1">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update - part 5
</commit_message>
<xml_diff>
--- a/data-input/data-quality/data-quality.xlsx
+++ b/data-input/data-quality/data-quality.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowaidakhaled/Documents/GitHub/wid-world/data-input/data-quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0419E511-53A3-7C45-B1DC-6AC89FCA56AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A837866-6FB5-DE43-B4D0-7BF0E5019C64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8300" yWindow="460" windowWidth="25300" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
   <si>
     <t>iso</t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>MO</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PG</t>
   </si>
 </sst>
 </file>
@@ -798,8 +804,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:B235" totalsRowShown="0">
-  <autoFilter ref="A1:B235" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:B237" totalsRowShown="0">
+  <autoFilter ref="A1:B237" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:B84">
     <sortCondition ref="A1:A84"/>
   </sortState>
@@ -1074,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B235"/>
+  <dimension ref="A1:B237"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+      <selection activeCell="B236" sqref="B236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2966,6 +2972,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B236" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B237" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>